<commit_message>
Uploading forecast for sprint 2
</commit_message>
<xml_diff>
--- a/Sprint2-docs/sprint2-burndown.xlsx
+++ b/Sprint2-docs/sprint2-burndown.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mbp13/Documents/GitHub/Team6-DatingApp/Sprint2-docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7F23A2E8-2DAA-AA4A-B3EE-3E2364CB5349}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41FEE13C-ECC3-2E4F-9E42-3C97C16B7597}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20000" yWindow="500" windowWidth="28800" windowHeight="16020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="51">
   <si>
     <t>Status</t>
   </si>
@@ -168,12 +168,6 @@
     <t>Sprint length (net)</t>
   </si>
   <si>
-    <t>20/03/22</t>
-  </si>
-  <si>
-    <t>27/03/22</t>
-  </si>
-  <si>
     <t>Reza</t>
   </si>
   <si>
@@ -207,7 +201,7 @@
     <numFmt numFmtId="165" formatCode="[$-407]d/\ mmm/\ yy;@"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -296,14 +290,8 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -338,12 +326,6 @@
       <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFB2CCDB"/>
-        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -433,7 +415,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -502,7 +484,6 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="13" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -520,6 +501,325 @@
     <dxf>
       <font>
         <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -562,45 +862,9 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -616,25 +880,6 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -645,24 +890,6 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -702,30 +929,6 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -735,30 +938,6 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -774,33 +953,14 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
         <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -815,33 +975,14 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
         <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -856,36 +997,6 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -897,142 +1008,12 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
         <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -1528,25 +1509,25 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1653,25 +1634,25 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>29</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>24.857142857142858</c:v>
+                  <c:v>10.285714285714286</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20.714285714285715</c:v>
+                  <c:v>8.5714285714285712</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16.571428571428569</c:v>
+                  <c:v>6.8571428571428577</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12.428571428571427</c:v>
+                  <c:v>5.1428571428571432</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.2857142857142847</c:v>
+                  <c:v>3.4285714285714288</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.1428571428571388</c:v>
+                  <c:v>1.7142857142857153</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -1782,25 +1763,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>29</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>29</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>29</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>21</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -4101,17 +4082,17 @@
     </filterColumn>
   </autoFilter>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Sprint ID" totalsRowLabel="Storypoints" dataDxfId="29" totalsRowDxfId="28"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Backlog Item ID" dataDxfId="27" totalsRowDxfId="26"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="StoryPoints" totalsRowFunction="sum" dataDxfId="25" totalsRowDxfId="24"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Story" dataDxfId="23" totalsRowDxfId="22"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Assigned to" dataDxfId="21" totalsRowDxfId="20"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="Status" dataDxfId="19" totalsRowDxfId="18"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Completed on" dataDxfId="17" totalsRowDxfId="16"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="Sprint day" dataDxfId="15" totalsRowDxfId="14">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Sprint ID" totalsRowLabel="Storypoints" dataDxfId="29" totalsRowDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Backlog Item ID" dataDxfId="28" totalsRowDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="StoryPoints" totalsRowFunction="sum" dataDxfId="27" totalsRowDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Story" dataDxfId="26" totalsRowDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Assigned to" dataDxfId="25" totalsRowDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="Status" dataDxfId="24" totalsRowDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Completed on" dataDxfId="23" totalsRowDxfId="7"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="Sprint day" dataDxfId="22" totalsRowDxfId="6">
       <calculatedColumnFormula>IF(ISBLANK(Backlog[[#This Row],[Completed on]]),"",Backlog[[#This Row],[Completed on]]-$C$1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0300-000009000000}" name="Help column" dataDxfId="13" totalsRowDxfId="12">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0300-000009000000}" name="Help column" dataDxfId="21" totalsRowDxfId="5">
       <calculatedColumnFormula>IF(ISBLANK(Backlog[[#This Row],[Completed on]]),"n","y")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4120,19 +4101,19 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Tabelle2" displayName="Tabelle2" ref="A3:E15" totalsRowCount="1" headerRowDxfId="11" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Tabelle2" displayName="Tabelle2" ref="A3:E15" totalsRowCount="1" headerRowDxfId="20" dataDxfId="19">
   <autoFilter ref="A3:E14" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Sprint day" totalsRowLabel="Outcome" dataDxfId="9" totalsRowDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Ideal line" dataDxfId="7" totalsRowDxfId="6">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Sprint day" totalsRowLabel="Outcome" dataDxfId="18" totalsRowDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Ideal line" dataDxfId="17" totalsRowDxfId="3">
       <calculatedColumnFormula>Backlog[[#Totals],[StoryPoints]]-(Backlog[[#Totals],[StoryPoints]]/Overview!$E$6*Tabelle2[[#This Row],[Sprint day]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Real course" dataDxfId="5" totalsRowDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Finished SP" totalsRowFunction="custom" dataDxfId="3" totalsRowDxfId="2">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Real course" dataDxfId="16" totalsRowDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Finished SP" totalsRowFunction="custom" dataDxfId="15" totalsRowDxfId="1">
       <calculatedColumnFormula>IF(Tabelle2[[#This Row],[Aktuell]]="y",SUMIF(Backlog[Sprint day],Tabelle2[[#This Row],[Sprint day]],Backlog[StoryPoints]),#N/A)</calculatedColumnFormula>
       <totalsRowFormula>SUMIFS(Tabelle2[Finished SP],Tabelle2[Finished SP],"&lt;&gt;#NV")</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="Aktuell" totalsRowFunction="count" dataDxfId="1" totalsRowDxfId="0">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="Aktuell" totalsRowFunction="count" dataDxfId="14" totalsRowDxfId="0">
       <calculatedColumnFormula>IF(NOW()&gt;=Backlog!$C$1+Tabelle2[[#This Row],[Sprint day]],"y","n")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4439,8 +4420,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AT58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="R42" sqref="R42"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4453,26 +4434,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:46" ht="98" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
-      <c r="L1" s="50"/>
-      <c r="M1" s="50"/>
-      <c r="N1" s="50"/>
-      <c r="O1" s="50"/>
-      <c r="P1" s="50"/>
-      <c r="Q1" s="50"/>
-      <c r="R1" s="50"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
+      <c r="K1" s="49"/>
+      <c r="L1" s="49"/>
+      <c r="M1" s="49"/>
+      <c r="N1" s="49"/>
+      <c r="O1" s="49"/>
+      <c r="P1" s="49"/>
+      <c r="Q1" s="49"/>
+      <c r="R1" s="49"/>
     </row>
     <row r="2" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A2" s="30"/>
@@ -4497,10 +4478,10 @@
         <v>13</v>
       </c>
       <c r="C3" s="30"/>
-      <c r="D3" s="49" t="s">
+      <c r="D3" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="49"/>
+      <c r="E3" s="48"/>
       <c r="F3" s="30"/>
       <c r="G3" s="30"/>
       <c r="H3" s="30"/>
@@ -4535,15 +4516,15 @@
       <c r="A5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="22" t="s">
-        <v>43</v>
+      <c r="B5" s="22">
+        <v>44661</v>
       </c>
       <c r="C5" s="28"/>
       <c r="D5" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="22" t="s">
-        <v>44</v>
+      <c r="E5" s="22">
+        <v>44668</v>
       </c>
       <c r="F5" s="28"/>
       <c r="G5" s="30"/>
@@ -4616,7 +4597,7 @@
         <v>26</v>
       </c>
       <c r="E8" s="21">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="F8" s="28"/>
       <c r="G8" s="28"/>
@@ -4640,7 +4621,7 @@
         <v>27</v>
       </c>
       <c r="E9" s="21">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F9" s="28"/>
       <c r="G9" s="28"/>
@@ -4661,10 +4642,10 @@
       </c>
       <c r="C10" s="33"/>
       <c r="D10" s="13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E10" s="21">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F10" s="28"/>
       <c r="G10" s="28"/>
@@ -4681,14 +4662,14 @@
         <v>22</v>
       </c>
       <c r="B11" s="23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C11" s="28"/>
       <c r="D11" s="13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E11" s="21">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F11" s="28"/>
       <c r="G11" s="28"/>
@@ -4863,7 +4844,7 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="26" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B22" s="30"/>
       <c r="C22" s="30"/>
@@ -4881,7 +4862,7 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="26" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B23" s="30"/>
       <c r="C23" s="30"/>
@@ -4899,7 +4880,7 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="26" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B24" s="30"/>
       <c r="C24" s="30"/>
@@ -4917,7 +4898,7 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="26" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B25" s="30"/>
       <c r="C25" s="30"/>
@@ -4935,7 +4916,7 @@
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="26" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B26" s="30"/>
       <c r="C26" s="30"/>
@@ -5215,7 +5196,7 @@
       <c r="M42" s="30"/>
       <c r="N42" s="30"/>
       <c r="R42" s="30" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.2">
@@ -5495,7 +5476,7 @@
   <dimension ref="A1:AK199"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="E172" sqref="E172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5515,9 +5496,9 @@
       <c r="B1" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="16" t="str">
+      <c r="C1" s="16">
         <f>Overview!$B$5</f>
-        <v>20/03/22</v>
+        <v>44661</v>
       </c>
       <c r="D1" s="28"/>
       <c r="E1" s="28"/>
@@ -5627,29 +5608,29 @@
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B6" s="2">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C6" s="2">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>30</v>
       </c>
       <c r="G6" s="15">
-        <v>44645</v>
-      </c>
-      <c r="H6" s="3" t="e">
-        <f>IF(ISBLANK(Backlog[[#This Row],[Completed on]]),"",Backlog[[#This Row],[Completed on]]-$C$1)</f>
-        <v>#VALUE!</v>
+        <v>44662</v>
+      </c>
+      <c r="H6" s="3">
+        <f>IF(ISBLANK(Backlog[[#This Row],[Completed on]]),"",Backlog[[#This Row],[Completed on]]-$C$1)</f>
+        <v>1</v>
       </c>
       <c r="I6" s="2" t="str">
         <f>IF(ISBLANK(Backlog[[#This Row],[Completed on]]),"n","y")</f>
@@ -5658,13 +5639,13 @@
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B7" s="2">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C7" s="2">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>9</v>
@@ -5676,11 +5657,11 @@
         <v>30</v>
       </c>
       <c r="G7" s="15">
-        <v>44647</v>
-      </c>
-      <c r="H7" s="3" t="e">
-        <f>IF(ISBLANK(Backlog[[#This Row],[Completed on]]),"",Backlog[[#This Row],[Completed on]]-$C$1)</f>
-        <v>#VALUE!</v>
+        <v>44664</v>
+      </c>
+      <c r="H7" s="3">
+        <f>IF(ISBLANK(Backlog[[#This Row],[Completed on]]),"",Backlog[[#This Row],[Completed on]]-$C$1)</f>
+        <v>3</v>
       </c>
       <c r="I7" s="2" t="str">
         <f>IF(ISBLANK(Backlog[[#This Row],[Completed on]]),"n","y")</f>
@@ -5689,29 +5670,29 @@
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B8" s="2">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C8" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>30</v>
       </c>
       <c r="G8" s="15">
-        <v>44644</v>
-      </c>
-      <c r="H8" s="3" t="e">
-        <f>IF(ISBLANK(Backlog[[#This Row],[Completed on]]),"",Backlog[[#This Row],[Completed on]]-$C$1)</f>
-        <v>#VALUE!</v>
+        <v>44666</v>
+      </c>
+      <c r="H8" s="3">
+        <f>IF(ISBLANK(Backlog[[#This Row],[Completed on]]),"",Backlog[[#This Row],[Completed on]]-$C$1)</f>
+        <v>5</v>
       </c>
       <c r="I8" s="2" t="str">
         <f>IF(ISBLANK(Backlog[[#This Row],[Completed on]]),"n","y")</f>
@@ -5720,29 +5701,29 @@
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B9" s="2">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="C9" s="2">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G9" s="48">
-        <v>44643</v>
-      </c>
-      <c r="H9" s="3" t="e">
-        <f>IF(ISBLANK(Backlog[[#This Row],[Completed on]]),"",Backlog[[#This Row],[Completed on]]-$C$1)</f>
-        <v>#VALUE!</v>
+      <c r="G9" s="15">
+        <v>44668</v>
+      </c>
+      <c r="H9" s="3">
+        <f>IF(ISBLANK(Backlog[[#This Row],[Completed on]]),"",Backlog[[#This Row],[Completed on]]-$C$1)</f>
+        <v>7</v>
       </c>
       <c r="I9" s="2" t="str">
         <f>IF(ISBLANK(Backlog[[#This Row],[Completed on]]),"n","y")</f>
@@ -8289,7 +8270,7 @@
       <c r="B160" s="42"/>
       <c r="C160" s="42">
         <f>SUBTOTAL(109,Backlog[StoryPoints])</f>
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="D160" s="42"/>
       <c r="E160" s="42"/>
@@ -8722,7 +8703,7 @@
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G6:G8" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G6:G9" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>43723</formula1>
     </dataValidation>
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B158 B5 B161:B1048576 B1" xr:uid="{00000000-0002-0000-0100-000001000000}">
@@ -8766,7 +8747,7 @@
   <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8785,11 +8766,11 @@
       <c r="E1" s="28"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
       <c r="D2" s="14"/>
       <c r="E2" s="2"/>
     </row>
@@ -8816,18 +8797,18 @@
       </c>
       <c r="B4" s="3">
         <f>Backlog[[#Totals],[StoryPoints]]-(Backlog[[#Totals],[StoryPoints]]/Overview!$E$6*Tabelle2[[#This Row],[Sprint day]])</f>
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="C4" s="2">
         <f>Backlog[[#Totals],[StoryPoints]]</f>
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="D4" s="2">
         <v>0</v>
       </c>
-      <c r="E4" s="2" t="e">
+      <c r="E4" s="2" t="str">
         <f ca="1">IF(NOW()&gt;=Backlog!$C$1+Tabelle2[[#This Row],[Sprint day]],"y","n")</f>
-        <v>#VALUE!</v>
+        <v>y</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -8836,17 +8817,17 @@
       </c>
       <c r="B5" s="3">
         <f>Backlog[[#Totals],[StoryPoints]]-(Backlog[[#Totals],[StoryPoints]]/Overview!$E$6*Tabelle2[[#This Row],[Sprint day]])</f>
-        <v>24.857142857142858</v>
+        <v>10.285714285714286</v>
       </c>
       <c r="C5" s="2">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="D5" s="2">
-        <v>0</v>
-      </c>
-      <c r="E5" s="2" t="e">
+        <v>5</v>
+      </c>
+      <c r="E5" s="2" t="str">
         <f ca="1">IF(NOW()&gt;=Backlog!$C$1+Tabelle2[[#This Row],[Sprint day]],"y","n")</f>
-        <v>#VALUE!</v>
+        <v>y</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -8855,18 +8836,17 @@
       </c>
       <c r="B6" s="3">
         <f>Backlog[[#Totals],[StoryPoints]]-(Backlog[[#Totals],[StoryPoints]]/Overview!$E$6*Tabelle2[[#This Row],[Sprint day]])</f>
-        <v>20.714285714285715</v>
+        <v>8.5714285714285712</v>
       </c>
       <c r="C6" s="2">
-        <f>C5-Tabelle2[[#This Row],[Finished SP]]</f>
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="D6" s="2">
         <v>0</v>
       </c>
-      <c r="E6" s="2" t="e">
+      <c r="E6" s="2" t="str">
         <f ca="1">IF(NOW()&gt;=Backlog!$C$1+Tabelle2[[#This Row],[Sprint day]],"y","n")</f>
-        <v>#VALUE!</v>
+        <v>y</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -8875,17 +8855,17 @@
       </c>
       <c r="B7" s="3">
         <f>Backlog[[#Totals],[StoryPoints]]-(Backlog[[#Totals],[StoryPoints]]/Overview!$E$6*Tabelle2[[#This Row],[Sprint day]])</f>
-        <v>16.571428571428569</v>
+        <v>6.8571428571428577</v>
       </c>
       <c r="C7" s="2">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="D7" s="2">
-        <v>8</v>
-      </c>
-      <c r="E7" s="2" t="e">
+        <v>2</v>
+      </c>
+      <c r="E7" s="2" t="str">
         <f ca="1">IF(NOW()&gt;=Backlog!$C$1+Tabelle2[[#This Row],[Sprint day]],"y","n")</f>
-        <v>#VALUE!</v>
+        <v>y</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -8894,18 +8874,17 @@
       </c>
       <c r="B8" s="3">
         <f>Backlog[[#Totals],[StoryPoints]]-(Backlog[[#Totals],[StoryPoints]]/Overview!$E$6*Tabelle2[[#This Row],[Sprint day]])</f>
-        <v>12.428571428571427</v>
+        <v>5.1428571428571432</v>
       </c>
       <c r="C8" s="2">
-        <f>C7-Tabelle2[[#This Row],[Finished SP]]</f>
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="D8" s="2">
-        <v>5</v>
-      </c>
-      <c r="E8" s="2" t="e">
+        <v>0</v>
+      </c>
+      <c r="E8" s="2" t="str">
         <f ca="1">IF(NOW()&gt;=Backlog!$C$1+Tabelle2[[#This Row],[Sprint day]],"y","n")</f>
-        <v>#VALUE!</v>
+        <v>y</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -8914,18 +8893,17 @@
       </c>
       <c r="B9" s="3">
         <f>Backlog[[#Totals],[StoryPoints]]-(Backlog[[#Totals],[StoryPoints]]/Overview!$E$6*Tabelle2[[#This Row],[Sprint day]])</f>
-        <v>8.2857142857142847</v>
+        <v>3.4285714285714288</v>
       </c>
       <c r="C9" s="2">
-        <f>C8-Tabelle2[[#This Row],[Finished SP]]</f>
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D9" s="2">
-        <v>8</v>
-      </c>
-      <c r="E9" s="2" t="e">
+        <v>2</v>
+      </c>
+      <c r="E9" s="2" t="str">
         <f ca="1">IF(NOW()&gt;=Backlog!$C$1+Tabelle2[[#This Row],[Sprint day]],"y","n")</f>
-        <v>#VALUE!</v>
+        <v>y</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -8934,18 +8912,17 @@
       </c>
       <c r="B10" s="3">
         <f>Backlog[[#Totals],[StoryPoints]]-(Backlog[[#Totals],[StoryPoints]]/Overview!$E$6*Tabelle2[[#This Row],[Sprint day]])</f>
-        <v>4.1428571428571388</v>
+        <v>1.7142857142857153</v>
       </c>
       <c r="C10" s="2">
-        <f>C9-Tabelle2[[#This Row],[Finished SP]]</f>
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D10" s="2">
         <v>0</v>
       </c>
-      <c r="E10" s="2" t="e">
+      <c r="E10" s="2" t="str">
         <f ca="1">IF(NOW()&gt;=Backlog!$C$1+Tabelle2[[#This Row],[Sprint day]],"y","n")</f>
-        <v>#VALUE!</v>
+        <v>y</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -8957,15 +8934,14 @@
         <v>0</v>
       </c>
       <c r="C11" s="2">
-        <f>C10-Tabelle2[[#This Row],[Finished SP]]</f>
         <v>0</v>
       </c>
       <c r="D11" s="2">
-        <v>8</v>
-      </c>
-      <c r="E11" s="2" t="e">
+        <v>3</v>
+      </c>
+      <c r="E11" s="2" t="str">
         <f ca="1">IF(NOW()&gt;=Backlog!$C$1+Tabelle2[[#This Row],[Sprint day]],"y","n")</f>
-        <v>#VALUE!</v>
+        <v>y</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -8973,9 +8949,9 @@
       <c r="B12" s="3"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
-      <c r="E12" s="2" t="e">
+      <c r="E12" s="2" t="str">
         <f ca="1">IF(NOW()&gt;=Backlog!$C$1+Tabelle2[[#This Row],[Sprint day]],"y","n")</f>
-        <v>#VALUE!</v>
+        <v>y</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -8983,9 +8959,9 @@
       <c r="B13" s="3"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
-      <c r="E13" s="2" t="e">
+      <c r="E13" s="2" t="str">
         <f ca="1">IF(NOW()&gt;=Backlog!$C$1+Tabelle2[[#This Row],[Sprint day]],"y","n")</f>
-        <v>#VALUE!</v>
+        <v>y</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -9003,7 +8979,7 @@
       <c r="C15" s="2"/>
       <c r="D15" s="2">
         <f>SUMIFS(Tabelle2[Finished SP],Tabelle2[Finished SP],"&lt;&gt;#NV")</f>
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="E15" s="2">
         <f ca="1">SUBTOTAL(103,Tabelle2[Aktuell])</f>

</xml_diff>